<commit_message>
practice set of excel sheet
</commit_message>
<xml_diff>
--- a/Excel files/Book1.xlsx
+++ b/Excel files/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium_Practice_Code_learning\Selenium_practice_code\Working_With_Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium_Practice_Code_learning\Selenium_practice_code\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46CDAFB-0839-4F51-BC5C-B164F09EEB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC984C0-AD50-4462-B80D-FA6695B41021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9120" xr2:uid="{035A2F95-9037-4B64-B159-3F3589AE9F6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035A2F95-9037-4B64-B159-3F3589AE9F6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>